<commit_message>
add option to change Fit plot xlab/ylab, translate default values (including Predict ylab), match default labels for fit/predict fixes #140 fixes #128 fixes #126
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D88F608-AF0F-904C-9AA7-A7479CDB1896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A7C73-0662-EC4D-890C-C6656EF35A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="28040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="33380" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - translations" sheetId="1" r:id="rId1"/>
@@ -552,6 +552,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">This webpage fits species sensitivity distributions to concentration data. The user is able to select more than one distribution and plot the individual fits. &lt;br/&gt;&lt;br/&gt;The columns in the goodness of fit table are the distribution (dist), the Anderson-Darling statistic (ad), the Kolmogorov-Smirnov statistic (ks), the Cramer-von Mises statistic (cvm), Akaike's Information Criterion (aic), Akaike's Information Criterion corrected for sample size (aicc), Bayesian Information Criterion (bic), the AICc difference (delta) and the AICc based Akaike weight (weight). The prediction is the model averaged (using aicc) estimate of the fit. The percent hazard concentration is the concentration of the chemical which is predicted to affect that percent of the species tested.&lt;br/&gt;&lt;br/&gt;To cite package ssdtools in publications use:&lt;br/&gt;Thorley, J. and Schwarz C., (2018). ssdtools: An R package to fit Species Sensitivity Distributions. Journal of Open Source Software, 3(31), 1082. </t>
     </r>
@@ -561,6 +562,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To</t>
     </r>
@@ -569,6 +571,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> cite the web app use:&lt;br/&gt;Seb Dalgarno (2018) ssdtools: A shiny web app to analyse species sensitivity distributions. Prepared by Poisson Consulting for the Ministry of the Environment, British Columbia. </t>
     </r>
@@ -578,6 +581,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>https://bcgov-env.shinyapps.io/ssdtools/</t>
     </r>
@@ -588,6 +592,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Cette page Web ajuste les fonctions de distribution de sensibilité des espèces aux données de concentration. L'utilisateur peut sélectionner plus d'une distribution et représenter individuellement chaque courbe d'ajustement dans un graphique. &lt;br/&gt;&lt;br/&gt; Les colonnes du tableau de l'évaluation de la qualité de l’ajustement des courbes de distributiont sont la distribution (dist), la statistique d’Anderson-Darling (ad), la statistique de Kolmogorov-Smirnov (ks), la statistique de Cramer-von-Mises (cmv), le critère d’information Akaike (aic), le critère d’information Akaike corrigé pour la taille de l’échantillon (aicc), le critère d’information Bayésien (bic), la différence entre AICc (delta) et la pondération des critères d'information AICc (coefficient de pondération). L’estimation de la fonction de distribution finale est basée sur l’inférence multimodèle (à partir de l’AICc). La concentration présentant un risque est la concentration estimée d’une substance affectant un centile (seuil) sélectionné de l’ensemble des espèces.&lt;br/&gt;&lt;br/&gt;Pour citer l’application R ‘ssdtools’:&lt;br/&gt;Thorley, J. and Schwarz C., (2018). ssdtools: An R package to fit Species Sensitivity Distributions. Journal of Open Source Software, 3(31), 1082. </t>
     </r>
@@ -597,6 +602,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour</t>
     </r>
@@ -605,6 +611,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> citer l’application web :&lt;br/&gt;Seb Dalgarno (2018) ssdtools: A shiny web app to analyse species sensitivity distributions. Prepared by Poisson Consulting for the Ministry of the Environment, British Columbia. </t>
     </r>
@@ -614,6 +621,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>https://bcgov-env.shinyapps.io/ssdtools/</t>
     </r>
@@ -739,14 +747,14 @@
     <t>Pourcentage d’espèces affectées</t>
   </si>
   <si>
-    <t xml:space="preserve">Species affected </t>
+    <t xml:space="preserve">Percent of species affected </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -757,12 +765,20 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -904,11 +920,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -917,25 +933,28 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2100,8 +2119,8 @@
   </sheetPr>
   <dimension ref="A1:IU78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2390,7 +2409,7 @@
       <c r="A26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="11" t="s">
         <v>217</v>
       </c>
       <c r="C26" s="8" t="s">

</xml_diff>

<commit_message>
change label of threshold %
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A7C73-0662-EC4D-890C-C6656EF35A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027FF127-54C9-CC4E-B0CF-9B691B67E608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="33380" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
   <si>
     <t>id</t>
   </si>
@@ -308,12 +308,6 @@
   </si>
   <si>
     <t>3thresh</t>
-  </si>
-  <si>
-    <t>Threshold (%)</t>
-  </si>
-  <si>
-    <t>Seuil (%)</t>
   </si>
   <si>
     <t>3samples</t>
@@ -748,6 +742,21 @@
   </si>
   <si>
     <t xml:space="preserve">Percent of species affected </t>
+  </si>
+  <si>
+    <t>Required estimate</t>
+  </si>
+  <si>
+    <t>Estimation requise</t>
+  </si>
+  <si>
+    <t>Seuil (%)</t>
+  </si>
+  <si>
+    <t>Threshold (%)</t>
+  </si>
+  <si>
+    <t>3threshlabel</t>
   </si>
 </sst>
 </file>
@@ -920,7 +929,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -955,6 +964,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2117,10 +2129,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU78"/>
+  <dimension ref="A1:IU79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2358,7 +2370,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2369,7 +2381,7 @@
         <v>63</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2410,10 +2422,10 @@
         <v>73</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2497,472 +2509,483 @@
       <c r="A34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>97</v>
+      <c r="B34" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>100</v>
+        <v>220</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>215</v>
+        <v>165</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
+    </row>
+    <row r="79" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B63" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C63" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
+    <hyperlink ref="B64" r:id="rId1" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;To" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C64" r:id="rId2" display="https://doi.org/10.21105/joss.01082&lt;br/&gt;&lt;br/&gt;Pour" xr:uid="{2EC433BA-6F80-AC4B-99E9-88803C6B48DF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
use 'Species affected (%)' as y-axis title, fixes #165
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8909F286-8F01-7F41-9904-86F5BAD8C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2CB40-C74C-2C4D-A8DC-2844BF3ECD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="33380" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -741,9 +741,6 @@
     <t>Pourcentage d’espèces affectées</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent of species affected </t>
-  </si>
-  <si>
     <t>Required estimate</t>
   </si>
   <si>
@@ -757,6 +754,9 @@
   </si>
   <si>
     <t>Fraction affectée</t>
+  </si>
+  <si>
+    <t>Species affected (%)</t>
   </si>
 </sst>
 </file>
@@ -2131,8 +2131,8 @@
   </sheetPr>
   <dimension ref="A1:IU79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2422,7 +2422,7 @@
         <v>73</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>214</v>
@@ -2510,21 +2510,21 @@
         <v>95</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
translations for required estimate input
</commit_message>
<xml_diff>
--- a/inst/extdata/translations.xlsx
+++ b/inst/extdata/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/shinyssdtools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2CB40-C74C-2C4D-A8DC-2844BF3ECD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC060C-530E-0E4F-8987-D760782E5360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="33380" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12480" yWindow="500" windowWidth="12460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - translations" sheetId="1" r:id="rId1"/>
@@ -744,9 +744,6 @@
     <t>Required estimate</t>
   </si>
   <si>
-    <t>Estimation requise</t>
-  </si>
-  <si>
     <t>3threshlabel</t>
   </si>
   <si>
@@ -757,13 +754,16 @@
   </si>
   <si>
     <t>Species affected (%)</t>
+  </si>
+  <si>
+    <t>Estimation nécessaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -788,6 +788,11 @@
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="4">
@@ -929,7 +934,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -968,6 +973,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2131,8 +2139,8 @@
   </sheetPr>
   <dimension ref="A1:IU79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2422,7 +2430,7 @@
         <v>73</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>214</v>
@@ -2510,21 +2518,21 @@
         <v>95</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>218</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>216</v>
+      <c r="C35" s="13" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>